<commit_message>
update changes in excel
</commit_message>
<xml_diff>
--- a/Bug and Task List.xlsx
+++ b/Bug and Task List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Detail</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Welcome E-mail template change</t>
+  </si>
+  <si>
+    <t>Correction of All masters page and complete CURD operation</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
   </si>
 </sst>
 </file>
@@ -431,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -581,7 +587,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -595,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -652,6 +658,20 @@
       </c>
       <c r="D15" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Tax and total amount related changes.
</commit_message>
<xml_diff>
--- a/Bug and Task List.xlsx
+++ b/Bug and Task List.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -559,7 +559,7 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>

<commit_message>
Update footer in project
</commit_message>
<xml_diff>
--- a/Bug and Task List.xlsx
+++ b/Bug and Task List.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Detail</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Changes in tax validation and implementation</t>
+  </si>
+  <si>
+    <t>CP1 Quality development</t>
   </si>
 </sst>
 </file>
@@ -440,11 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -479,7 +484,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -493,7 +498,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -507,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -521,10 +526,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -538,7 +543,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -552,7 +557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -608,7 +613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -633,7 +638,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -647,10 +652,10 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -678,15 +683,40 @@
         <v>24</v>
       </c>
     </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D16">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="In-Progress"/>
-        <filter val="Pending"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update latest script and excel file
</commit_message>
<xml_diff>
--- a/Bug and Task List.xlsx
+++ b/Bug and Task List.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="37">
   <si>
     <t>Detail</t>
   </si>
@@ -105,6 +105,30 @@
   </si>
   <si>
     <t>Dashboard development</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>sunil</t>
+  </si>
+  <si>
+    <t>saswat</t>
+  </si>
+  <si>
+    <t>nitin</t>
+  </si>
+  <si>
+    <t>Payment Email and SMS text implementation</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Aakash</t>
+  </si>
+  <si>
+    <t>Email template and sms text is pending from SNPL end</t>
   </si>
 </sst>
 </file>
@@ -452,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -463,9 +487,11 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -478,8 +504,11 @@
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -492,8 +521,11 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,8 +538,11 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -520,8 +555,11 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -534,8 +572,11 @@
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -548,8 +589,11 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -562,8 +606,11 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -576,8 +623,11 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -590,8 +640,11 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -604,8 +657,11 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -618,8 +674,11 @@
       <c r="D11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -632,8 +691,11 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -646,8 +708,11 @@
       <c r="D13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -658,10 +723,13 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -674,8 +742,11 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -688,8 +759,11 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -702,8 +776,11 @@
       <c r="D17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -716,8 +793,11 @@
       <c r="D18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
@@ -730,8 +810,11 @@
       <c r="D19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -743,6 +826,29 @@
       </c>
       <c r="D20" t="s">
         <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>